<commit_message>
api - change url
</commit_message>
<xml_diff>
--- a/doc/interface/api.xlsx
+++ b/doc/interface/api.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="-80" yWindow="-24440" windowWidth="38400" windowHeight="24000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="meetings" sheetId="1" r:id="rId1"/>
     <sheet name="bookings" sheetId="2" r:id="rId2"/>
-    <sheet name="users" sheetId="3" r:id="rId3"/>
+    <sheet name="users" sheetId="4" r:id="rId3"/>
+    <sheet name="auths" sheetId="3" r:id="rId4"/>
+    <sheet name="message" sheetId="5" r:id="rId5"/>
+    <sheet name="lookups" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="157">
   <si>
     <t>function type</t>
   </si>
@@ -51,9 +54,6 @@
   </si>
   <si>
     <t>GET</t>
-  </si>
-  <si>
-    <t>/meetings</t>
   </si>
   <si>
     <t>cityId</t>
@@ -135,33 +135,12 @@
     <t>meetings.updateTime</t>
   </si>
   <si>
-    <t>meetings.sellerUser</t>
-  </si>
-  <si>
     <t>object</t>
   </si>
   <si>
-    <t>meetings.sellerUser.id</t>
-  </si>
-  <si>
-    <t>meetings.sellerUser.name</t>
-  </si>
-  <si>
-    <t>meetings.sellerUser.title</t>
-  </si>
-  <si>
-    <t>meetings.sellerUser.icon</t>
-  </si>
-  <si>
-    <t>meetings.sellerUser.rating</t>
-  </si>
-  <si>
     <t>get meeting</t>
   </si>
   <si>
-    <t>/meetings/${meetingId}</t>
-  </si>
-  <si>
     <t>example</t>
   </si>
   <si>
@@ -192,30 +171,6 @@
     <t>meeting.updateTime</t>
   </si>
   <si>
-    <t>meeting.calender</t>
-  </si>
-  <si>
-    <t>meeting.calender.fromTime</t>
-  </si>
-  <si>
-    <t>meeting.calender.toTime</t>
-  </si>
-  <si>
-    <t>meeting.location.address</t>
-  </si>
-  <si>
-    <t>meeting.location.gps</t>
-  </si>
-  <si>
-    <t>meeting.location</t>
-  </si>
-  <si>
-    <t>meeting.calender.id</t>
-  </si>
-  <si>
-    <t>meeting.location.id</t>
-  </si>
-  <si>
     <t>PUT</t>
   </si>
   <si>
@@ -240,9 +195,6 @@
     <t>get bookings</t>
   </si>
   <si>
-    <t>/bookings</t>
-  </si>
-  <si>
     <t>bookings</t>
   </si>
   <si>
@@ -285,9 +237,6 @@
     <t>meeting.seller.rating</t>
   </si>
   <si>
-    <t>meeting.location.cityId</t>
-  </si>
-  <si>
     <t>insert</t>
   </si>
   <si>
@@ -295,6 +244,279 @@
   </si>
   <si>
     <t>remove</t>
+  </si>
+  <si>
+    <t>api/v1/meetings/${meetingId}</t>
+  </si>
+  <si>
+    <t>api/v1/meetings</t>
+  </si>
+  <si>
+    <t>pageNum</t>
+  </si>
+  <si>
+    <t>delete meeting</t>
+  </si>
+  <si>
+    <t>book meeting</t>
+  </si>
+  <si>
+    <t>api/v1/meetings/${meetingId}/actions/booking</t>
+  </si>
+  <si>
+    <t>meetingId</t>
+  </si>
+  <si>
+    <t>calenderId</t>
+  </si>
+  <si>
+    <t>locationId</t>
+  </si>
+  <si>
+    <t>api/v1/bookings</t>
+  </si>
+  <si>
+    <t>bookings.meetings.id</t>
+  </si>
+  <si>
+    <t>bookings.meetings.subject</t>
+  </si>
+  <si>
+    <t>bookings.seller</t>
+  </si>
+  <si>
+    <t>bookings.seller.id</t>
+  </si>
+  <si>
+    <t>bookings.seller.name</t>
+  </si>
+  <si>
+    <t>bookings.seller.icon</t>
+  </si>
+  <si>
+    <t>bookings.buyer</t>
+  </si>
+  <si>
+    <t>bookings.buyer.id</t>
+  </si>
+  <si>
+    <t>bookings.buyer.name</t>
+  </si>
+  <si>
+    <t>bookings.buyer.icon</t>
+  </si>
+  <si>
+    <t>bookings.calender</t>
+  </si>
+  <si>
+    <t>bookings.calender.id</t>
+  </si>
+  <si>
+    <t>bookings.calender.fromTime</t>
+  </si>
+  <si>
+    <t>bookings.calender.toTime</t>
+  </si>
+  <si>
+    <t>bookings.location</t>
+  </si>
+  <si>
+    <t>bookings.location.id</t>
+  </si>
+  <si>
+    <t>bookings.location.cityId</t>
+  </si>
+  <si>
+    <t>bookings.location.address</t>
+  </si>
+  <si>
+    <t>bookings.location.gps</t>
+  </si>
+  <si>
+    <t>bookings.createTime</t>
+  </si>
+  <si>
+    <t>bookings.updateTime</t>
+  </si>
+  <si>
+    <t>bookings.status</t>
+  </si>
+  <si>
+    <t>get booking</t>
+  </si>
+  <si>
+    <t>api/v1/bookings/${bookingId}</t>
+  </si>
+  <si>
+    <t>bookings.meetings.target</t>
+  </si>
+  <si>
+    <t>bookings.meetings.desc</t>
+  </si>
+  <si>
+    <t>bookings.meetings.price</t>
+  </si>
+  <si>
+    <t>bookings.meetings.createTime</t>
+  </si>
+  <si>
+    <t>bookings.meetings.updateTime</t>
+  </si>
+  <si>
+    <t>accept booking</t>
+  </si>
+  <si>
+    <t>api/v1/bookings/${bookingId}/actions/accept</t>
+  </si>
+  <si>
+    <t>bookingId</t>
+  </si>
+  <si>
+    <t>reject booking</t>
+  </si>
+  <si>
+    <t>api/v1/bookings/${bookingId}/actions/reject</t>
+  </si>
+  <si>
+    <t>cancel booking</t>
+  </si>
+  <si>
+    <t>api/v1/bookings/${bookingId}/actions/cancel</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>logoff</t>
+  </si>
+  <si>
+    <t>register</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email verify</t>
+  </si>
+  <si>
+    <t>api/v1/register</t>
+  </si>
+  <si>
+    <t>api/v1/login</t>
+  </si>
+  <si>
+    <t>api/v1/logoff</t>
+  </si>
+  <si>
+    <t>get user</t>
+  </si>
+  <si>
+    <t>api/v1/users/${userId}</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>user.name</t>
+  </si>
+  <si>
+    <t>user.icon</t>
+  </si>
+  <si>
+    <t>user.phone</t>
+  </si>
+  <si>
+    <t>user.email</t>
+  </si>
+  <si>
+    <t>user.gender</t>
+  </si>
+  <si>
+    <t>user.jobTitle</t>
+  </si>
+  <si>
+    <t>user.desc</t>
+  </si>
+  <si>
+    <t>user.rating</t>
+  </si>
+  <si>
+    <t>user.createTime</t>
+  </si>
+  <si>
+    <t>user.updateTime</t>
+  </si>
+  <si>
+    <t>update user</t>
+  </si>
+  <si>
+    <t>comment booking</t>
+  </si>
+  <si>
+    <t>api/v1/booking/${bookingId}/actions/comment</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>comment.rating</t>
+  </si>
+  <si>
+    <t>comment.content</t>
+  </si>
+  <si>
+    <t>meeting.comments</t>
+  </si>
+  <si>
+    <t>meeting.calenders</t>
+  </si>
+  <si>
+    <t>meeting.calenders.id</t>
+  </si>
+  <si>
+    <t>meeting.calenders.fromTime</t>
+  </si>
+  <si>
+    <t>meeting.calenders.toTime</t>
+  </si>
+  <si>
+    <t>meeting.locations</t>
+  </si>
+  <si>
+    <t>meeting.locations.id</t>
+  </si>
+  <si>
+    <t>meeting.locations.cityId</t>
+  </si>
+  <si>
+    <t>meeting.locations.address</t>
+  </si>
+  <si>
+    <t>meeting.locations.gps</t>
+  </si>
+  <si>
+    <t>meeting.comments.rating</t>
+  </si>
+  <si>
+    <t>meeting.comments.content</t>
+  </si>
+  <si>
+    <t>meeting.comments.user</t>
+  </si>
+  <si>
+    <t>meeting.comments.user.id</t>
+  </si>
+  <si>
+    <t>meeting.comments.user.icon</t>
+  </si>
+  <si>
+    <t>meeting.comments.user.name</t>
   </si>
 </sst>
 </file>
@@ -423,7 +645,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="178">
+  <cellStyleXfs count="344">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -586,6 +808,172 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -613,7 +1001,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="159"/>
   </cellXfs>
-  <cellStyles count="178">
+  <cellStyles count="344">
     <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
     <cellStyle name="Bad" xfId="160" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -702,6 +1090,89 @@
     <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="277" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="279" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="281" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="283" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="285" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="287" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="289" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="291" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="293" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="295" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="297" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="299" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="301" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="303" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="305" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="307" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="309" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="311" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="313" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="315" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="317" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="319" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="321" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="323" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="325" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="327" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="329" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="331" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="333" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="335" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="337" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="339" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="341" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="343" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="159" builtinId="26"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -790,6 +1261,89 @@
     <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="270" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="272" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="274" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="276" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="278" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="280" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="282" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="284" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="286" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="288" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="290" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="292" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="294" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="296" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="298" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="300" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="302" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="304" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="306" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="308" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="310" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="312" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="314" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="316" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="318" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="320" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="322" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="324" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="326" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="328" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="330" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="332" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="334" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="336" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="338" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="340" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="342" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="161" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1120,23 +1674,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M94"/>
+  <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G60" sqref="E60:G60"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="8.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="17" thickBot="1">
@@ -1144,7 +1699,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1168,7 +1723,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="M1" s="6"/>
     </row>
@@ -1180,100 +1735,100 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="D3" t="s">
+      <c r="E3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
       <c r="G4" t="b">
         <v>0</v>
       </c>
-      <c r="M4" s="7" t="s">
-        <v>82</v>
+      <c r="M4" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="E5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>83</v>
+      <c r="M5" s="7" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="E6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" t="s">
-        <v>24</v>
+        <v>0</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="E7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="E8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
@@ -1281,10 +1836,10 @@
     </row>
     <row r="9" spans="1:13">
       <c r="E9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -1292,10 +1847,10 @@
     </row>
     <row r="10" spans="1:13">
       <c r="E10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
@@ -1303,10 +1858,10 @@
     </row>
     <row r="11" spans="1:13">
       <c r="E11" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="G11" t="b">
         <v>0</v>
@@ -1314,10 +1869,10 @@
     </row>
     <row r="12" spans="1:13">
       <c r="E12" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="G12" t="b">
         <v>0</v>
@@ -1325,10 +1880,10 @@
     </row>
     <row r="13" spans="1:13">
       <c r="E13" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G13" t="b">
         <v>0</v>
@@ -1336,10 +1891,10 @@
     </row>
     <row r="14" spans="1:13">
       <c r="E14" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
@@ -1347,10 +1902,10 @@
     </row>
     <row r="15" spans="1:13">
       <c r="E15" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
@@ -1358,64 +1913,64 @@
     </row>
     <row r="16" spans="1:13">
       <c r="E16" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="F16" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G16" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
         <v>9</v>
       </c>
-      <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="D20" t="s">
         <v>15</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="D19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" t="s">
-        <v>31</v>
-      </c>
-      <c r="G19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
       <c r="E20" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="G20" t="b">
         <v>0</v>
@@ -1423,10 +1978,10 @@
     </row>
     <row r="21" spans="1:10">
       <c r="E21" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="F21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G21" t="b">
         <v>0</v>
@@ -1434,35 +1989,35 @@
     </row>
     <row r="22" spans="1:10">
       <c r="E22" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G22" t="b">
-        <v>1</v>
-      </c>
-      <c r="H22" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="E23" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G23" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="E24" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F24" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G24" t="b">
         <v>0</v>
@@ -1470,10 +2025,10 @@
     </row>
     <row r="25" spans="1:10">
       <c r="E25" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
@@ -1481,10 +2036,10 @@
     </row>
     <row r="26" spans="1:10">
       <c r="E26" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G26" t="b">
         <v>0</v>
@@ -1492,10 +2047,10 @@
     </row>
     <row r="27" spans="1:10">
       <c r="E27" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="F27" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="G27" t="b">
         <v>0</v>
@@ -1503,10 +2058,10 @@
     </row>
     <row r="28" spans="1:10">
       <c r="E28" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="F28" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="G28" t="b">
         <v>0</v>
@@ -1514,10 +2069,10 @@
     </row>
     <row r="29" spans="1:10">
       <c r="E29" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="F29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G29" t="b">
         <v>0</v>
@@ -1525,10 +2080,10 @@
     </row>
     <row r="30" spans="1:10">
       <c r="E30" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="F30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G30" t="b">
         <v>0</v>
@@ -1536,10 +2091,10 @@
     </row>
     <row r="31" spans="1:10">
       <c r="E31" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="F31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G31" t="b">
         <v>0</v>
@@ -1547,40 +2102,40 @@
     </row>
     <row r="32" spans="1:10">
       <c r="E32" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="F32" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G32" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="5:7">
       <c r="E33" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="F33" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G33" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="5:7">
       <c r="E34" t="s">
-        <v>55</v>
+        <v>142</v>
       </c>
       <c r="F34" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G34" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="5:7">
       <c r="E35" t="s">
-        <v>50</v>
+        <v>143</v>
       </c>
       <c r="F35" t="s">
         <v>20</v>
@@ -1589,376 +2144,360 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="5:7">
       <c r="E36" t="s">
-        <v>51</v>
+        <v>144</v>
       </c>
       <c r="F36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G36" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="5:7">
       <c r="E37" t="s">
-        <v>54</v>
+        <v>145</v>
       </c>
       <c r="F37" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G37" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="5:7">
       <c r="E38" t="s">
-        <v>56</v>
+        <v>146</v>
       </c>
       <c r="F38" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G38" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
-      <c r="E39" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G39" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="E40" t="s">
-        <v>52</v>
-      </c>
-      <c r="F40" t="s">
-        <v>21</v>
-      </c>
-      <c r="G40" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
+    <row r="39" spans="5:7">
+      <c r="E39" t="s">
+        <v>147</v>
+      </c>
+      <c r="F39" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="5:7">
+      <c r="E40" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G40" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="5:7">
       <c r="E41" t="s">
-        <v>53</v>
+        <v>149</v>
       </c>
       <c r="F41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G41" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" t="s">
+    <row r="42" spans="5:7">
+      <c r="E42" t="s">
+        <v>150</v>
+      </c>
+      <c r="F42" t="s">
+        <v>20</v>
+      </c>
+      <c r="G42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="5:7">
+      <c r="E43" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="5:7">
+      <c r="E44" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="5:7">
+      <c r="E45" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="5:7">
+      <c r="E46" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G46" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="5:7">
+      <c r="E47" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G47" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="5:7">
+      <c r="E48" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="E49" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G49" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" t="s">
+        <v>67</v>
+      </c>
+      <c r="D51" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" t="s">
+        <v>33</v>
+      </c>
+      <c r="F51" t="s">
+        <v>29</v>
+      </c>
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="E52" t="s">
+        <v>35</v>
+      </c>
+      <c r="F52" t="s">
+        <v>20</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="E53" t="s">
+        <v>36</v>
+      </c>
+      <c r="F53" t="s">
+        <v>20</v>
+      </c>
+      <c r="G53" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="E54" t="s">
+        <v>37</v>
+      </c>
+      <c r="F54" t="s">
+        <v>20</v>
+      </c>
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="E55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F55" t="s">
+        <v>26</v>
+      </c>
+      <c r="G55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="E56" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G56" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="E57" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G57" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="E58" t="s">
+        <v>57</v>
+      </c>
+      <c r="F58" t="s">
+        <v>29</v>
+      </c>
+      <c r="G58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="E59" t="s">
         <v>58</v>
       </c>
-      <c r="B43" t="s">
-        <v>57</v>
-      </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" t="s">
-        <v>15</v>
-      </c>
-      <c r="E43" t="s">
-        <v>41</v>
-      </c>
-      <c r="F43" t="s">
-        <v>31</v>
-      </c>
-      <c r="G43" t="b">
-        <v>0</v>
-      </c>
-      <c r="J43" s="1"/>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="E44" t="s">
-        <v>43</v>
-      </c>
-      <c r="F44" t="s">
-        <v>21</v>
-      </c>
-      <c r="G44" t="b">
-        <v>0</v>
-      </c>
-      <c r="J44" s="1"/>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="E45" t="s">
-        <v>44</v>
-      </c>
-      <c r="F45" t="s">
-        <v>21</v>
-      </c>
-      <c r="G45" t="b">
-        <v>1</v>
-      </c>
-      <c r="H45" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="E46" t="s">
-        <v>45</v>
-      </c>
-      <c r="F46" t="s">
-        <v>21</v>
-      </c>
-      <c r="G46" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="E47" t="s">
-        <v>46</v>
-      </c>
-      <c r="F47" t="s">
-        <v>27</v>
-      </c>
-      <c r="G47" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="E48" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G48" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="4:7">
-      <c r="E49" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G49" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="4:7">
-      <c r="E50" t="s">
-        <v>74</v>
-      </c>
-      <c r="F50" t="s">
-        <v>31</v>
-      </c>
-      <c r="G50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="4:7">
-      <c r="E51" t="s">
-        <v>75</v>
-      </c>
-      <c r="F51" t="s">
-        <v>21</v>
-      </c>
-      <c r="G51" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="4:7">
-      <c r="E52" t="s">
-        <v>76</v>
-      </c>
-      <c r="F52" t="s">
-        <v>21</v>
-      </c>
-      <c r="G52" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="4:7">
-      <c r="E53" t="s">
-        <v>77</v>
-      </c>
-      <c r="F53" t="s">
-        <v>21</v>
-      </c>
-      <c r="G53" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="4:7">
-      <c r="E54" t="s">
-        <v>78</v>
-      </c>
-      <c r="F54" t="s">
-        <v>21</v>
-      </c>
-      <c r="G54" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="4:7">
-      <c r="E55" t="s">
-        <v>79</v>
-      </c>
-      <c r="F55" t="s">
-        <v>12</v>
-      </c>
-      <c r="G55" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="4:7">
-      <c r="E56" t="s">
-        <v>49</v>
-      </c>
-      <c r="F56" t="s">
-        <v>18</v>
-      </c>
-      <c r="G56" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="4:7">
-      <c r="E57" t="s">
-        <v>50</v>
-      </c>
-      <c r="F57" t="s">
-        <v>20</v>
-      </c>
-      <c r="G57" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="4:7">
-      <c r="E58" t="s">
-        <v>51</v>
-      </c>
-      <c r="F58" t="s">
-        <v>20</v>
-      </c>
-      <c r="G58" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="4:7">
-      <c r="E59" t="s">
-        <v>54</v>
-      </c>
       <c r="F59" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G59" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="4:7">
-      <c r="E60" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G60" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="4:7">
+    <row r="60" spans="1:10">
+      <c r="E60" t="s">
+        <v>59</v>
+      </c>
+      <c r="F60" t="s">
+        <v>20</v>
+      </c>
+      <c r="G60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="E61" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="F61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G61" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="4:7">
+    <row r="62" spans="1:10">
       <c r="E62" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F62" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G62" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="4:7">
-      <c r="D63" t="s">
-        <v>16</v>
-      </c>
+    <row r="63" spans="1:10">
       <c r="E63" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F63" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G63" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="4:7">
+    <row r="64" spans="1:10">
       <c r="E64" t="s">
-        <v>60</v>
+        <v>142</v>
       </c>
       <c r="F64" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G64" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:10">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
-      <c r="J65" s="3"/>
+      <c r="E65" t="s">
+        <v>144</v>
+      </c>
+      <c r="F65" t="s">
+        <v>19</v>
+      </c>
+      <c r="G65" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="66" spans="1:10">
-      <c r="A66" t="s">
-        <v>61</v>
-      </c>
-      <c r="B66" t="s">
-        <v>62</v>
-      </c>
-      <c r="C66" t="s">
-        <v>38</v>
-      </c>
-      <c r="D66" t="s">
-        <v>15</v>
-      </c>
       <c r="E66" t="s">
-        <v>41</v>
+        <v>145</v>
       </c>
       <c r="F66" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="G66" t="b">
         <v>0</v>
@@ -1966,90 +2505,103 @@
     </row>
     <row r="67" spans="1:10">
       <c r="E67" t="s">
-        <v>42</v>
+        <v>146</v>
       </c>
       <c r="F67" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G67" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:10">
-      <c r="E68" t="s">
-        <v>43</v>
-      </c>
-      <c r="F68" t="s">
-        <v>21</v>
-      </c>
-      <c r="G68" t="b">
+      <c r="E68" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G68" s="5" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="E69" t="s">
-        <v>44</v>
+        <v>149</v>
       </c>
       <c r="F69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G69" t="b">
-        <v>1</v>
-      </c>
-      <c r="H69" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="E70" t="s">
+        <v>150</v>
+      </c>
+      <c r="F70" t="s">
+        <v>20</v>
+      </c>
+      <c r="G70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="D71" t="s">
+        <v>15</v>
+      </c>
+      <c r="E71" t="s">
+        <v>43</v>
+      </c>
+      <c r="F71" t="s">
+        <v>11</v>
+      </c>
+      <c r="G71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="E72" t="s">
+        <v>44</v>
+      </c>
+      <c r="F72" t="s">
+        <v>20</v>
+      </c>
+      <c r="G72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" t="s">
         <v>45</v>
       </c>
-      <c r="F70" t="s">
-        <v>21</v>
-      </c>
-      <c r="G70" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
-      <c r="E71" t="s">
+      <c r="B74" t="s">
         <v>46</v>
       </c>
-      <c r="F71" t="s">
-        <v>27</v>
-      </c>
-      <c r="G71" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10">
-      <c r="E72" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G72" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10">
-      <c r="E73" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G73" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10">
+      <c r="C74" t="s">
+        <v>66</v>
+      </c>
+      <c r="D74" t="s">
+        <v>14</v>
+      </c>
       <c r="E74" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="F74" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G74" t="b">
         <v>0</v>
@@ -2057,10 +2609,10 @@
     </row>
     <row r="75" spans="1:10">
       <c r="E75" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="F75" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G75" t="b">
         <v>0</v>
@@ -2068,10 +2620,10 @@
     </row>
     <row r="76" spans="1:10">
       <c r="E76" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="F76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G76" t="b">
         <v>0</v>
@@ -2079,21 +2631,24 @@
     </row>
     <row r="77" spans="1:10">
       <c r="E77" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="F77" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G77" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H77" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="E78" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="F78" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G78" t="b">
         <v>0</v>
@@ -2101,51 +2656,51 @@
     </row>
     <row r="79" spans="1:10">
       <c r="E79" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="F79" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="G79" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:10">
-      <c r="E80" t="s">
-        <v>49</v>
-      </c>
-      <c r="F80" t="s">
-        <v>18</v>
-      </c>
-      <c r="G80" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10">
-      <c r="E81" t="s">
-        <v>55</v>
-      </c>
-      <c r="F81" t="s">
-        <v>21</v>
-      </c>
-      <c r="G81" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10">
+      <c r="E80" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G80" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="5:7">
+      <c r="E81" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G81" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="5:7">
       <c r="E82" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F82" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G82" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="5:7">
       <c r="E83" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F83" t="s">
         <v>20</v>
@@ -2154,137 +2709,318 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="5:7">
       <c r="E84" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F84" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G84" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="5:7">
       <c r="E85" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F85" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G85" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="5:7">
       <c r="E86" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="F86" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G86" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="5:7">
       <c r="E87" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="F87" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="G87" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
-      <c r="D88" t="s">
-        <v>16</v>
-      </c>
+    <row r="88" spans="5:7">
       <c r="E88" t="s">
-        <v>59</v>
+        <v>142</v>
       </c>
       <c r="F88" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G88" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
-      <c r="E89" t="s">
-        <v>60</v>
-      </c>
-      <c r="F89" t="s">
-        <v>21</v>
-      </c>
-      <c r="G89" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10">
-      <c r="A90" s="3"/>
-      <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
-      <c r="E90" s="3"/>
-      <c r="F90" s="3"/>
-      <c r="G90" s="3"/>
-      <c r="H90" s="3"/>
-      <c r="I90" s="3"/>
-      <c r="J90" s="3"/>
-    </row>
-    <row r="91" spans="1:10">
-      <c r="A91" t="s">
-        <v>61</v>
-      </c>
-      <c r="B91" t="s">
-        <v>63</v>
-      </c>
-      <c r="C91" t="s">
-        <v>38</v>
-      </c>
-      <c r="D91" t="s">
+    <row r="89" spans="5:7">
+      <c r="E89" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G89" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="5:7">
+      <c r="E90" t="s">
+        <v>144</v>
+      </c>
+      <c r="F90" t="s">
+        <v>19</v>
+      </c>
+      <c r="G90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="5:7">
+      <c r="E91" t="s">
+        <v>145</v>
+      </c>
+      <c r="F91" t="s">
+        <v>19</v>
+      </c>
+      <c r="G91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="5:7">
+      <c r="E92" t="s">
+        <v>146</v>
+      </c>
+      <c r="F92" t="s">
+        <v>17</v>
+      </c>
+      <c r="G92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="5:7">
+      <c r="E93" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G93" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="5:7">
+      <c r="E94" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G94" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="5:7">
+      <c r="E95" t="s">
+        <v>149</v>
+      </c>
+      <c r="F95" t="s">
+        <v>20</v>
+      </c>
+      <c r="G95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="5:7">
+      <c r="E96" t="s">
+        <v>150</v>
+      </c>
+      <c r="F96" t="s">
+        <v>20</v>
+      </c>
+      <c r="G96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="D97" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="92" spans="1:10">
-      <c r="D92" t="s">
-        <v>16</v>
-      </c>
-      <c r="E92" t="s">
-        <v>59</v>
-      </c>
-      <c r="F92" t="s">
-        <v>12</v>
-      </c>
-      <c r="G92" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10">
-      <c r="E93" t="s">
-        <v>60</v>
-      </c>
-      <c r="F93" t="s">
-        <v>21</v>
-      </c>
-      <c r="G93" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10">
-      <c r="A94" s="3"/>
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
-      <c r="E94" s="3"/>
-      <c r="F94" s="3"/>
-      <c r="G94" s="3"/>
-      <c r="H94" s="3"/>
-      <c r="I94" s="3"/>
-      <c r="J94" s="3"/>
+      <c r="E97" t="s">
+        <v>43</v>
+      </c>
+      <c r="F97" t="s">
+        <v>11</v>
+      </c>
+      <c r="G97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="E98" t="s">
+        <v>44</v>
+      </c>
+      <c r="F98" t="s">
+        <v>20</v>
+      </c>
+      <c r="G98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" s="3"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+      <c r="G99" s="3"/>
+      <c r="H99" s="3"/>
+      <c r="I99" s="3"/>
+      <c r="J99" s="3"/>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" t="s">
+        <v>69</v>
+      </c>
+      <c r="B100" t="s">
+        <v>47</v>
+      </c>
+      <c r="C100" t="s">
+        <v>66</v>
+      </c>
+      <c r="D100" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="D101" t="s">
+        <v>15</v>
+      </c>
+      <c r="E101" t="s">
+        <v>43</v>
+      </c>
+      <c r="F101" t="s">
+        <v>11</v>
+      </c>
+      <c r="G101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="E102" t="s">
+        <v>44</v>
+      </c>
+      <c r="F102" t="s">
+        <v>20</v>
+      </c>
+      <c r="G102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103" s="3"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
+      <c r="I103" s="3"/>
+      <c r="J103" s="3"/>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104" t="s">
+        <v>70</v>
+      </c>
+      <c r="B104" t="s">
+        <v>41</v>
+      </c>
+      <c r="C104" t="s">
+        <v>71</v>
+      </c>
+      <c r="D104" t="s">
+        <v>14</v>
+      </c>
+      <c r="E104" t="s">
+        <v>72</v>
+      </c>
+      <c r="F104" t="s">
+        <v>20</v>
+      </c>
+      <c r="G104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="E105" t="s">
+        <v>73</v>
+      </c>
+      <c r="F105" t="s">
+        <v>20</v>
+      </c>
+      <c r="G105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="E106" t="s">
+        <v>74</v>
+      </c>
+      <c r="F106" t="s">
+        <v>20</v>
+      </c>
+      <c r="G106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10">
+      <c r="D107" t="s">
+        <v>15</v>
+      </c>
+      <c r="E107" t="s">
+        <v>43</v>
+      </c>
+      <c r="F107" t="s">
+        <v>11</v>
+      </c>
+      <c r="G107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10">
+      <c r="E108" t="s">
+        <v>44</v>
+      </c>
+      <c r="F108" t="s">
+        <v>20</v>
+      </c>
+      <c r="G108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109" s="3"/>
+      <c r="B109" s="3"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="3"/>
+      <c r="F109" s="3"/>
+      <c r="G109" s="3"/>
+      <c r="H109" s="3"/>
+      <c r="I109" s="3"/>
+      <c r="J109" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2299,21 +3035,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
   </cols>
@@ -2323,7 +3060,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -2347,32 +3084,41 @@
         <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16" thickTop="1">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -2380,15 +3126,21 @@
     </row>
     <row r="4" spans="1:10">
       <c r="E4" t="s">
-        <v>67</v>
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="E5" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -2396,10 +3148,10 @@
     </row>
     <row r="6" spans="1:10">
       <c r="E6" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
@@ -2407,24 +3159,21 @@
     </row>
     <row r="7" spans="1:10">
       <c r="E7" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="E8" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
@@ -2432,10 +3181,10 @@
     </row>
     <row r="9" spans="1:10">
       <c r="E9" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -2443,7 +3192,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="E10" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
@@ -2454,7 +3203,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="E11" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
@@ -2465,10 +3214,10 @@
     </row>
     <row r="12" spans="1:10">
       <c r="E12" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G12" t="b">
         <v>0</v>
@@ -2476,10 +3225,10 @@
     </row>
     <row r="13" spans="1:10">
       <c r="E13" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G13" t="b">
         <v>0</v>
@@ -2487,10 +3236,10 @@
     </row>
     <row r="14" spans="1:10">
       <c r="E14" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
@@ -2498,10 +3247,10 @@
     </row>
     <row r="15" spans="1:10">
       <c r="E15" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
@@ -2509,10 +3258,10 @@
     </row>
     <row r="16" spans="1:10">
       <c r="E16" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="G16" t="b">
         <v>0</v>
@@ -2520,26 +3269,746 @@
     </row>
     <row r="17" spans="1:10">
       <c r="E17" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G17" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="E18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="E19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="E20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="E21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="E22" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="E23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="E25" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="E26" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="E27" t="s">
+        <v>97</v>
+      </c>
+      <c r="F27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="E31" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="E32" t="s">
+        <v>76</v>
+      </c>
+      <c r="F32" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7">
+      <c r="E33" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="5:7">
+      <c r="E34" t="s">
+        <v>100</v>
+      </c>
+      <c r="F34" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7">
+      <c r="E35" t="s">
+        <v>101</v>
+      </c>
+      <c r="F35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7">
+      <c r="E36" t="s">
+        <v>102</v>
+      </c>
+      <c r="F36" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7">
+      <c r="E37" t="s">
+        <v>103</v>
+      </c>
+      <c r="F37" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7">
+      <c r="E38" t="s">
+        <v>104</v>
+      </c>
+      <c r="F38" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="5:7">
+      <c r="E39" t="s">
+        <v>78</v>
+      </c>
+      <c r="F39" t="s">
+        <v>29</v>
+      </c>
+      <c r="G39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="5:7">
+      <c r="E40" t="s">
+        <v>79</v>
+      </c>
+      <c r="F40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="5:7">
+      <c r="E41" t="s">
+        <v>80</v>
+      </c>
+      <c r="F41" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="5:7">
+      <c r="E42" t="s">
+        <v>81</v>
+      </c>
+      <c r="F42" t="s">
+        <v>20</v>
+      </c>
+      <c r="G42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="5:7">
+      <c r="E43" t="s">
+        <v>82</v>
+      </c>
+      <c r="F43" t="s">
+        <v>29</v>
+      </c>
+      <c r="G43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="5:7">
+      <c r="E44" t="s">
+        <v>83</v>
+      </c>
+      <c r="F44" t="s">
+        <v>20</v>
+      </c>
+      <c r="G44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="5:7">
+      <c r="E45" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="5:7">
+      <c r="E46" t="s">
+        <v>85</v>
+      </c>
+      <c r="F46" t="s">
+        <v>20</v>
+      </c>
+      <c r="G46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="5:7">
+      <c r="E47" t="s">
+        <v>86</v>
+      </c>
+      <c r="F47" t="s">
+        <v>29</v>
+      </c>
+      <c r="G47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="5:7">
+      <c r="E48" t="s">
+        <v>87</v>
+      </c>
+      <c r="F48" t="s">
+        <v>20</v>
+      </c>
+      <c r="G48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="E49" t="s">
+        <v>88</v>
+      </c>
+      <c r="F49" t="s">
+        <v>19</v>
+      </c>
+      <c r="G49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="E50" t="s">
+        <v>89</v>
+      </c>
+      <c r="F50" t="s">
+        <v>19</v>
+      </c>
+      <c r="G50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="E51" t="s">
+        <v>90</v>
+      </c>
+      <c r="F51" t="s">
+        <v>29</v>
+      </c>
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="E52" t="s">
+        <v>91</v>
+      </c>
+      <c r="F52" t="s">
+        <v>20</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="E53" t="s">
+        <v>92</v>
+      </c>
+      <c r="F53" t="s">
+        <v>20</v>
+      </c>
+      <c r="G53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="E54" t="s">
+        <v>93</v>
+      </c>
+      <c r="F54" t="s">
+        <v>20</v>
+      </c>
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="E55" t="s">
+        <v>94</v>
+      </c>
+      <c r="F55" t="s">
+        <v>20</v>
+      </c>
+      <c r="G55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="E56" t="s">
+        <v>95</v>
+      </c>
+      <c r="F56" t="s">
+        <v>19</v>
+      </c>
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="E57" t="s">
+        <v>96</v>
+      </c>
+      <c r="F57" t="s">
+        <v>19</v>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="E58" t="s">
+        <v>97</v>
+      </c>
+      <c r="F58" t="s">
+        <v>20</v>
+      </c>
+      <c r="G58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" t="s">
+        <v>105</v>
+      </c>
+      <c r="B60" t="s">
+        <v>46</v>
+      </c>
+      <c r="C60" t="s">
+        <v>106</v>
+      </c>
+      <c r="D60" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" t="s">
+        <v>107</v>
+      </c>
+      <c r="F60" t="s">
+        <v>20</v>
+      </c>
+      <c r="G60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="D61" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" t="s">
+        <v>43</v>
+      </c>
+      <c r="F61" t="s">
+        <v>11</v>
+      </c>
+      <c r="G61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="E62" t="s">
+        <v>44</v>
+      </c>
+      <c r="F62" t="s">
+        <v>20</v>
+      </c>
+      <c r="G62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" t="s">
+        <v>108</v>
+      </c>
+      <c r="B64" t="s">
+        <v>46</v>
+      </c>
+      <c r="C64" t="s">
+        <v>109</v>
+      </c>
+      <c r="D64" t="s">
+        <v>14</v>
+      </c>
+      <c r="E64" t="s">
+        <v>107</v>
+      </c>
+      <c r="F64" t="s">
+        <v>20</v>
+      </c>
+      <c r="G64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="D65" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65" t="s">
+        <v>43</v>
+      </c>
+      <c r="F65" t="s">
+        <v>11</v>
+      </c>
+      <c r="G65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="E66" t="s">
+        <v>44</v>
+      </c>
+      <c r="F66" t="s">
+        <v>20</v>
+      </c>
+      <c r="G66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" t="s">
+        <v>110</v>
+      </c>
+      <c r="B68" t="s">
+        <v>46</v>
+      </c>
+      <c r="C68" t="s">
+        <v>111</v>
+      </c>
+      <c r="D68" t="s">
+        <v>14</v>
+      </c>
+      <c r="E68" t="s">
+        <v>107</v>
+      </c>
+      <c r="F68" t="s">
+        <v>20</v>
+      </c>
+      <c r="G68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="D69" t="s">
+        <v>15</v>
+      </c>
+      <c r="E69" t="s">
+        <v>43</v>
+      </c>
+      <c r="F69" t="s">
+        <v>11</v>
+      </c>
+      <c r="G69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="E70" t="s">
+        <v>44</v>
+      </c>
+      <c r="F70" t="s">
+        <v>20</v>
+      </c>
+      <c r="G70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" t="s">
+        <v>136</v>
+      </c>
+      <c r="B72" t="s">
+        <v>41</v>
+      </c>
+      <c r="C72" t="s">
+        <v>137</v>
+      </c>
+      <c r="D72" t="s">
+        <v>14</v>
+      </c>
+      <c r="E72" t="s">
+        <v>138</v>
+      </c>
+      <c r="F72" t="s">
+        <v>29</v>
+      </c>
+      <c r="G72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="E73" t="s">
+        <v>139</v>
+      </c>
+      <c r="F73" t="s">
+        <v>11</v>
+      </c>
+      <c r="G73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="E74" t="s">
+        <v>140</v>
+      </c>
+      <c r="F74" t="s">
+        <v>20</v>
+      </c>
+      <c r="G74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="D75" t="s">
+        <v>15</v>
+      </c>
+      <c r="E75" t="s">
+        <v>43</v>
+      </c>
+      <c r="F75" t="s">
+        <v>11</v>
+      </c>
+      <c r="G75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="E76" t="s">
+        <v>44</v>
+      </c>
+      <c r="F76" t="s">
+        <v>20</v>
+      </c>
+      <c r="G76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+      <c r="J77" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2553,6 +4022,641 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="17" thickBot="1">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16" thickTop="1">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="E4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="E5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="E6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="E7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="E8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="E9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="E10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="E11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="E12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="E13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="E16" t="s">
+        <v>125</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="E17" t="s">
+        <v>126</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="E18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="E19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="E20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="E21" t="s">
+        <v>130</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="E22" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="E23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection sqref="A1:J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="17" thickBot="1">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16" thickTop="1">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="E3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="E4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="E9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2567,4 +4671,23 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
make some change...   city id change to meeting level
</commit_message>
<xml_diff>
--- a/doc/interface/api.xlsx
+++ b/doc/interface/api.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-24440" windowWidth="38400" windowHeight="24000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="14060" yWindow="-24000" windowWidth="38400" windowHeight="23540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="meetings" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="157">
   <si>
     <t>function type</t>
   </si>
@@ -120,9 +120,6 @@
     <t>""</t>
   </si>
   <si>
-    <t>meetings.desc</t>
-  </si>
-  <si>
     <t>meetings.price</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>meeting.target</t>
   </si>
   <si>
-    <t>meeting.desc</t>
-  </si>
-  <si>
     <t>meeting.price</t>
   </si>
   <si>
@@ -492,9 +486,6 @@
     <t>meeting.locations.id</t>
   </si>
   <si>
-    <t>meeting.locations.cityId</t>
-  </si>
-  <si>
     <t>meeting.locations.address</t>
   </si>
   <si>
@@ -517,13 +508,22 @@
   </si>
   <si>
     <t>meeting.comments.user.name</t>
+  </si>
+  <si>
+    <t>meetings.description</t>
+  </si>
+  <si>
+    <t>meeting.description</t>
+  </si>
+  <si>
+    <t>meeting.cityId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -597,6 +597,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -991,7 +999,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
@@ -1000,6 +1008,7 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="161"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="159"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="344">
     <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
@@ -1674,10 +1683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M109"/>
+  <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1723,7 +1732,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M1" s="6"/>
     </row>
@@ -1735,7 +1744,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -1754,13 +1763,13 @@
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="E3" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="5" t="b">
+      <c r="G3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1778,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1792,7 +1801,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1806,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1825,7 +1834,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="E8" t="s">
-        <v>24</v>
+        <v>154</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
@@ -1836,10 +1845,10 @@
     </row>
     <row r="9" spans="1:13">
       <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
         <v>25</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -1847,7 +1856,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="E10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
@@ -1858,7 +1867,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="E11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" t="s">
         <v>19</v>
@@ -1869,10 +1878,10 @@
     </row>
     <row r="12" spans="1:13">
       <c r="E12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" t="b">
         <v>0</v>
@@ -1880,7 +1889,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="E13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
         <v>20</v>
@@ -1891,7 +1900,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="E14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
         <v>20</v>
@@ -1902,7 +1911,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="E15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F15" t="s">
         <v>20</v>
@@ -1913,7 +1922,7 @@
     </row>
     <row r="16" spans="1:13">
       <c r="E16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
         <v>20</v>
@@ -1924,7 +1933,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="E17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F17" t="s">
         <v>11</v>
@@ -1947,19 +1956,19 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1967,10 +1976,10 @@
         <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G20" t="b">
         <v>0</v>
@@ -1978,7 +1987,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="E21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F21" t="s">
         <v>20</v>
@@ -1989,7 +1998,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="E22" t="s">
-        <v>35</v>
+        <v>156</v>
       </c>
       <c r="F22" t="s">
         <v>20</v>
@@ -2000,35 +2009,35 @@
     </row>
     <row r="23" spans="1:10">
       <c r="E23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F23" t="s">
         <v>20</v>
       </c>
       <c r="G23" t="b">
-        <v>1</v>
-      </c>
-      <c r="H23" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="E24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F24" t="s">
         <v>20</v>
       </c>
       <c r="G24" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="E25" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="F25" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
@@ -2036,10 +2045,10 @@
     </row>
     <row r="26" spans="1:10">
       <c r="E26" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F26" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G26" t="b">
         <v>0</v>
@@ -2047,7 +2056,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="E27" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F27" t="s">
         <v>19</v>
@@ -2058,10 +2067,10 @@
     </row>
     <row r="28" spans="1:10">
       <c r="E28" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="F28" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G28" t="b">
         <v>0</v>
@@ -2069,10 +2078,10 @@
     </row>
     <row r="29" spans="1:10">
       <c r="E29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F29" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G29" t="b">
         <v>0</v>
@@ -2080,7 +2089,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="E30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F30" t="s">
         <v>20</v>
@@ -2091,7 +2100,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="E31" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F31" t="s">
         <v>20</v>
@@ -2102,7 +2111,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="E32" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F32" t="s">
         <v>20</v>
@@ -2111,53 +2120,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="5:7">
+    <row r="33" spans="3:7">
       <c r="E33" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7">
+      <c r="E34" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" t="s">
         <v>11</v>
       </c>
-      <c r="G33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="5:7">
-      <c r="E34" t="s">
+      <c r="G34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7">
+      <c r="E35" t="s">
+        <v>140</v>
+      </c>
+      <c r="F35" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7">
+      <c r="C36" s="8"/>
+      <c r="E36" t="s">
+        <v>141</v>
+      </c>
+      <c r="F36" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7">
+      <c r="E37" t="s">
         <v>142</v>
-      </c>
-      <c r="F34" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="5:7">
-      <c r="E35" t="s">
-        <v>143</v>
-      </c>
-      <c r="F35" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="5:7">
-      <c r="E36" t="s">
-        <v>144</v>
-      </c>
-      <c r="F36" t="s">
-        <v>19</v>
-      </c>
-      <c r="G36" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="5:7">
-      <c r="E37" t="s">
-        <v>145</v>
       </c>
       <c r="F37" t="s">
         <v>19</v>
@@ -2166,135 +2176,135 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="5:7">
+    <row r="38" spans="3:7">
       <c r="E38" t="s">
+        <v>143</v>
+      </c>
+      <c r="F38" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7">
+      <c r="E39" t="s">
+        <v>144</v>
+      </c>
+      <c r="F39" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7">
+      <c r="E40" t="s">
+        <v>145</v>
+      </c>
+      <c r="F40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7">
+      <c r="E41" t="s">
         <v>146</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F41" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7">
+      <c r="E42" t="s">
+        <v>147</v>
+      </c>
+      <c r="F42" t="s">
+        <v>20</v>
+      </c>
+      <c r="G42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7">
+      <c r="E43" t="s">
+        <v>139</v>
+      </c>
+      <c r="F43" t="s">
         <v>17</v>
       </c>
-      <c r="G38" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="5:7">
-      <c r="E39" t="s">
-        <v>147</v>
-      </c>
-      <c r="F39" t="s">
-        <v>20</v>
-      </c>
-      <c r="G39" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="5:7">
-      <c r="E40" s="5" t="s">
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7">
+      <c r="E44" t="s">
+        <v>150</v>
+      </c>
+      <c r="F44" t="s">
+        <v>28</v>
+      </c>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7">
+      <c r="E45" t="s">
+        <v>151</v>
+      </c>
+      <c r="F45" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7">
+      <c r="E46" t="s">
+        <v>152</v>
+      </c>
+      <c r="F46" t="s">
+        <v>20</v>
+      </c>
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7">
+      <c r="E47" t="s">
+        <v>153</v>
+      </c>
+      <c r="F47" t="s">
+        <v>20</v>
+      </c>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7">
+      <c r="E48" t="s">
         <v>148</v>
       </c>
-      <c r="F40" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G40" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="5:7">
-      <c r="E41" t="s">
+      <c r="F48" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="E49" t="s">
         <v>149</v>
       </c>
-      <c r="F41" t="s">
-        <v>20</v>
-      </c>
-      <c r="G41" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="5:7">
-      <c r="E42" t="s">
-        <v>150</v>
-      </c>
-      <c r="F42" t="s">
-        <v>20</v>
-      </c>
-      <c r="G42" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="5:7">
-      <c r="E43" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G43" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="5:7">
-      <c r="E44" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G44" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="5:7">
-      <c r="E45" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G45" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="5:7">
-      <c r="E46" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G46" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="5:7">
-      <c r="E47" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G47" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="5:7">
-      <c r="E48" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G48" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
-      <c r="E49" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G49" s="5" t="b">
+      <c r="F49" t="s">
+        <v>20</v>
+      </c>
+      <c r="G49" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2312,22 +2322,22 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C51" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D51" t="s">
         <v>14</v>
       </c>
       <c r="E51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F51" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G51" t="b">
         <v>0</v>
@@ -2336,7 +2346,7 @@
     </row>
     <row r="52" spans="1:10">
       <c r="E52" t="s">
-        <v>35</v>
+        <v>156</v>
       </c>
       <c r="F52" t="s">
         <v>20</v>
@@ -2348,68 +2358,69 @@
     </row>
     <row r="53" spans="1:10">
       <c r="E53" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F53" t="s">
         <v>20</v>
       </c>
       <c r="G53" t="b">
-        <v>1</v>
-      </c>
-      <c r="H53" t="s">
-        <v>23</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J53" s="1"/>
     </row>
     <row r="54" spans="1:10">
       <c r="E54" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F54" t="s">
         <v>20</v>
       </c>
       <c r="G54" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H54" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="E55" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="F55" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G55" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:10">
-      <c r="E56" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G56" s="4" t="b">
+      <c r="E56" t="s">
+        <v>36</v>
+      </c>
+      <c r="F56" t="s">
+        <v>25</v>
+      </c>
+      <c r="G56" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:10">
-      <c r="E57" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G57" s="4" t="b">
+      <c r="E57" t="s">
+        <v>55</v>
+      </c>
+      <c r="F57" t="s">
+        <v>28</v>
+      </c>
+      <c r="G57" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="E58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F58" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G58" t="b">
         <v>0</v>
@@ -2417,7 +2428,7 @@
     </row>
     <row r="59" spans="1:10">
       <c r="E59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F59" t="s">
         <v>20</v>
@@ -2428,7 +2439,7 @@
     </row>
     <row r="60" spans="1:10">
       <c r="E60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F60" t="s">
         <v>20</v>
@@ -2439,7 +2450,7 @@
     </row>
     <row r="61" spans="1:10">
       <c r="E61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F61" t="s">
         <v>20</v>
@@ -2450,10 +2461,10 @@
     </row>
     <row r="62" spans="1:10">
       <c r="E62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F62" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G62" t="b">
         <v>0</v>
@@ -2461,10 +2472,10 @@
     </row>
     <row r="63" spans="1:10">
       <c r="E63" t="s">
-        <v>62</v>
+        <v>140</v>
       </c>
       <c r="F63" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G63" t="b">
         <v>0</v>
@@ -2475,7 +2486,7 @@
         <v>142</v>
       </c>
       <c r="F64" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G64" t="b">
         <v>0</v>
@@ -2483,7 +2494,7 @@
     </row>
     <row r="65" spans="1:10">
       <c r="E65" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F65" t="s">
         <v>19</v>
@@ -2494,10 +2505,10 @@
     </row>
     <row r="66" spans="1:10">
       <c r="E66" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F66" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G66" t="b">
         <v>0</v>
@@ -2508,29 +2519,32 @@
         <v>146</v>
       </c>
       <c r="F67" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G67" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:10">
-      <c r="E68" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G68" s="5" t="b">
+      <c r="E68" t="s">
+        <v>147</v>
+      </c>
+      <c r="F68" t="s">
+        <v>20</v>
+      </c>
+      <c r="G68" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:10">
+      <c r="D69" t="s">
+        <v>15</v>
+      </c>
       <c r="E69" t="s">
-        <v>149</v>
+        <v>41</v>
       </c>
       <c r="F69" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G69" t="b">
         <v>0</v>
@@ -2538,7 +2552,7 @@
     </row>
     <row r="70" spans="1:10">
       <c r="E70" t="s">
-        <v>150</v>
+        <v>42</v>
       </c>
       <c r="F70" t="s">
         <v>20</v>
@@ -2548,60 +2562,57 @@
       </c>
     </row>
     <row r="71" spans="1:10">
-      <c r="D71" t="s">
-        <v>15</v>
-      </c>
-      <c r="E71" t="s">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" t="s">
         <v>43</v>
       </c>
-      <c r="F71" t="s">
-        <v>11</v>
-      </c>
-      <c r="G71" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10">
+      <c r="B72" t="s">
+        <v>44</v>
+      </c>
+      <c r="C72" t="s">
+        <v>64</v>
+      </c>
+      <c r="D72" t="s">
+        <v>14</v>
+      </c>
       <c r="E72" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F72" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G72" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:10">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
-      <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
-      <c r="J73" s="3"/>
+      <c r="E73" t="s">
+        <v>33</v>
+      </c>
+      <c r="F73" t="s">
+        <v>20</v>
+      </c>
+      <c r="G73" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="74" spans="1:10">
-      <c r="A74" t="s">
-        <v>45</v>
-      </c>
-      <c r="B74" t="s">
-        <v>46</v>
-      </c>
-      <c r="C74" t="s">
-        <v>66</v>
-      </c>
-      <c r="D74" t="s">
-        <v>14</v>
-      </c>
       <c r="E74" t="s">
-        <v>33</v>
+        <v>156</v>
       </c>
       <c r="F74" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G74" t="b">
         <v>0</v>
@@ -2626,29 +2637,29 @@
         <v>20</v>
       </c>
       <c r="G76" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H76" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="E77" t="s">
-        <v>36</v>
+        <v>155</v>
       </c>
       <c r="F77" t="s">
         <v>20</v>
       </c>
       <c r="G77" t="b">
-        <v>1</v>
-      </c>
-      <c r="H77" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="E78" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F78" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G78" t="b">
         <v>0</v>
@@ -2656,194 +2667,220 @@
     </row>
     <row r="79" spans="1:10">
       <c r="E79" t="s">
-        <v>38</v>
+        <v>140</v>
       </c>
       <c r="F79" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="G79" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:10">
-      <c r="E80" s="4" t="s">
+      <c r="E80" t="s">
+        <v>142</v>
+      </c>
+      <c r="F80" t="s">
+        <v>19</v>
+      </c>
+      <c r="G80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="E81" t="s">
+        <v>143</v>
+      </c>
+      <c r="F81" t="s">
+        <v>19</v>
+      </c>
+      <c r="G81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="E82" t="s">
+        <v>144</v>
+      </c>
+      <c r="F82" t="s">
+        <v>17</v>
+      </c>
+      <c r="G82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="E83" t="s">
+        <v>146</v>
+      </c>
+      <c r="F83" t="s">
+        <v>20</v>
+      </c>
+      <c r="G83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="E84" t="s">
+        <v>147</v>
+      </c>
+      <c r="F84" t="s">
+        <v>20</v>
+      </c>
+      <c r="G84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="D85" t="s">
+        <v>15</v>
+      </c>
+      <c r="E85" t="s">
+        <v>41</v>
+      </c>
+      <c r="F85" t="s">
+        <v>11</v>
+      </c>
+      <c r="G85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="E86" t="s">
+        <v>42</v>
+      </c>
+      <c r="F86" t="s">
+        <v>20</v>
+      </c>
+      <c r="G86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" s="3"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="3"/>
+      <c r="I87" s="3"/>
+      <c r="J87" s="3"/>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88" t="s">
+        <v>67</v>
+      </c>
+      <c r="B88" t="s">
+        <v>45</v>
+      </c>
+      <c r="C88" t="s">
+        <v>64</v>
+      </c>
+      <c r="D88" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="D89" t="s">
+        <v>15</v>
+      </c>
+      <c r="E89" t="s">
+        <v>41</v>
+      </c>
+      <c r="F89" t="s">
+        <v>11</v>
+      </c>
+      <c r="G89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="E90" t="s">
+        <v>42</v>
+      </c>
+      <c r="F90" t="s">
+        <v>20</v>
+      </c>
+      <c r="G90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" t="s">
+        <v>68</v>
+      </c>
+      <c r="B92" t="s">
         <v>39</v>
       </c>
-      <c r="F80" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G80" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="5:7">
-      <c r="E81" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F81" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G81" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="5:7">
-      <c r="E82" t="s">
-        <v>57</v>
-      </c>
-      <c r="F82" t="s">
-        <v>29</v>
-      </c>
-      <c r="G82" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="5:7">
-      <c r="E83" t="s">
-        <v>58</v>
-      </c>
-      <c r="F83" t="s">
-        <v>20</v>
-      </c>
-      <c r="G83" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="5:7">
-      <c r="E84" t="s">
-        <v>59</v>
-      </c>
-      <c r="F84" t="s">
-        <v>20</v>
-      </c>
-      <c r="G84" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="5:7">
-      <c r="E85" t="s">
-        <v>60</v>
-      </c>
-      <c r="F85" t="s">
-        <v>20</v>
-      </c>
-      <c r="G85" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="5:7">
-      <c r="E86" t="s">
-        <v>61</v>
-      </c>
-      <c r="F86" t="s">
-        <v>20</v>
-      </c>
-      <c r="G86" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="5:7">
-      <c r="E87" t="s">
-        <v>62</v>
-      </c>
-      <c r="F87" t="s">
+      <c r="C92" t="s">
+        <v>69</v>
+      </c>
+      <c r="D92" t="s">
+        <v>14</v>
+      </c>
+      <c r="E92" t="s">
+        <v>70</v>
+      </c>
+      <c r="F92" t="s">
+        <v>20</v>
+      </c>
+      <c r="G92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="E93" t="s">
+        <v>71</v>
+      </c>
+      <c r="F93" t="s">
+        <v>20</v>
+      </c>
+      <c r="G93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="E94" t="s">
+        <v>72</v>
+      </c>
+      <c r="F94" t="s">
+        <v>20</v>
+      </c>
+      <c r="G94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="D95" t="s">
+        <v>15</v>
+      </c>
+      <c r="E95" t="s">
+        <v>41</v>
+      </c>
+      <c r="F95" t="s">
         <v>11</v>
       </c>
-      <c r="G87" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="5:7">
-      <c r="E88" t="s">
-        <v>142</v>
-      </c>
-      <c r="F88" t="s">
-        <v>17</v>
-      </c>
-      <c r="G88" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="5:7">
-      <c r="E89" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F89" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G89" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="5:7">
-      <c r="E90" t="s">
-        <v>144</v>
-      </c>
-      <c r="F90" t="s">
-        <v>19</v>
-      </c>
-      <c r="G90" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="5:7">
-      <c r="E91" t="s">
-        <v>145</v>
-      </c>
-      <c r="F91" t="s">
-        <v>19</v>
-      </c>
-      <c r="G91" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="5:7">
-      <c r="E92" t="s">
-        <v>146</v>
-      </c>
-      <c r="F92" t="s">
-        <v>17</v>
-      </c>
-      <c r="G92" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="5:7">
-      <c r="E93" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="F93" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G93" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="5:7">
-      <c r="E94" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="F94" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G94" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="5:7">
-      <c r="E95" t="s">
-        <v>149</v>
-      </c>
-      <c r="F95" t="s">
-        <v>20</v>
-      </c>
       <c r="G95" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="5:7">
+    <row r="96" spans="1:10">
       <c r="E96" t="s">
-        <v>150</v>
+        <v>42</v>
       </c>
       <c r="F96" t="s">
         <v>20</v>
@@ -2853,174 +2890,16 @@
       </c>
     </row>
     <row r="97" spans="1:10">
-      <c r="D97" t="s">
-        <v>15</v>
-      </c>
-      <c r="E97" t="s">
-        <v>43</v>
-      </c>
-      <c r="F97" t="s">
-        <v>11</v>
-      </c>
-      <c r="G97" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10">
-      <c r="E98" t="s">
-        <v>44</v>
-      </c>
-      <c r="F98" t="s">
-        <v>20</v>
-      </c>
-      <c r="G98" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10">
-      <c r="A99" s="3"/>
-      <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
-      <c r="E99" s="3"/>
-      <c r="F99" s="3"/>
-      <c r="G99" s="3"/>
-      <c r="H99" s="3"/>
-      <c r="I99" s="3"/>
-      <c r="J99" s="3"/>
-    </row>
-    <row r="100" spans="1:10">
-      <c r="A100" t="s">
-        <v>69</v>
-      </c>
-      <c r="B100" t="s">
-        <v>47</v>
-      </c>
-      <c r="C100" t="s">
-        <v>66</v>
-      </c>
-      <c r="D100" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10">
-      <c r="D101" t="s">
-        <v>15</v>
-      </c>
-      <c r="E101" t="s">
-        <v>43</v>
-      </c>
-      <c r="F101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G101" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10">
-      <c r="E102" t="s">
-        <v>44</v>
-      </c>
-      <c r="F102" t="s">
-        <v>20</v>
-      </c>
-      <c r="G102" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10">
-      <c r="A103" s="3"/>
-      <c r="B103" s="3"/>
-      <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
-      <c r="E103" s="3"/>
-      <c r="F103" s="3"/>
-      <c r="G103" s="3"/>
-      <c r="H103" s="3"/>
-      <c r="I103" s="3"/>
-      <c r="J103" s="3"/>
-    </row>
-    <row r="104" spans="1:10">
-      <c r="A104" t="s">
-        <v>70</v>
-      </c>
-      <c r="B104" t="s">
-        <v>41</v>
-      </c>
-      <c r="C104" t="s">
-        <v>71</v>
-      </c>
-      <c r="D104" t="s">
-        <v>14</v>
-      </c>
-      <c r="E104" t="s">
-        <v>72</v>
-      </c>
-      <c r="F104" t="s">
-        <v>20</v>
-      </c>
-      <c r="G104" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10">
-      <c r="E105" t="s">
-        <v>73</v>
-      </c>
-      <c r="F105" t="s">
-        <v>20</v>
-      </c>
-      <c r="G105" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10">
-      <c r="E106" t="s">
-        <v>74</v>
-      </c>
-      <c r="F106" t="s">
-        <v>20</v>
-      </c>
-      <c r="G106" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10">
-      <c r="D107" t="s">
-        <v>15</v>
-      </c>
-      <c r="E107" t="s">
-        <v>43</v>
-      </c>
-      <c r="F107" t="s">
-        <v>11</v>
-      </c>
-      <c r="G107" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10">
-      <c r="E108" t="s">
-        <v>44</v>
-      </c>
-      <c r="F108" t="s">
-        <v>20</v>
-      </c>
-      <c r="G108" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10">
-      <c r="A109" s="3"/>
-      <c r="B109" s="3"/>
-      <c r="C109" s="3"/>
-      <c r="D109" s="3"/>
-      <c r="E109" s="3"/>
-      <c r="F109" s="3"/>
-      <c r="G109" s="3"/>
-      <c r="H109" s="3"/>
-      <c r="I109" s="3"/>
-      <c r="J109" s="3"/>
+      <c r="A97" s="3"/>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="3"/>
+      <c r="I97" s="3"/>
+      <c r="J97" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3037,7 +2916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A36" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
@@ -3084,24 +2963,24 @@
         <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16" thickTop="1">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -3115,7 +2994,7 @@
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -3126,10 +3005,10 @@
     </row>
     <row r="4" spans="1:10">
       <c r="E4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>
@@ -3137,7 +3016,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="E5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
@@ -3148,7 +3027,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="E6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
@@ -3159,10 +3038,10 @@
     </row>
     <row r="7" spans="1:10">
       <c r="E7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -3170,10 +3049,10 @@
     </row>
     <row r="8" spans="1:10">
       <c r="E8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
@@ -3181,7 +3060,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="E9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
@@ -3192,7 +3071,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="E10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
@@ -3203,7 +3082,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="E11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
@@ -3214,10 +3093,10 @@
     </row>
     <row r="12" spans="1:10">
       <c r="E12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" t="b">
         <v>0</v>
@@ -3225,7 +3104,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="E13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F13" t="s">
         <v>20</v>
@@ -3236,7 +3115,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="E14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F14" t="s">
         <v>20</v>
@@ -3247,7 +3126,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="E15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F15" t="s">
         <v>20</v>
@@ -3258,10 +3137,10 @@
     </row>
     <row r="16" spans="1:10">
       <c r="E16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G16" t="b">
         <v>0</v>
@@ -3269,7 +3148,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="E17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F17" t="s">
         <v>20</v>
@@ -3280,7 +3159,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="E18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F18" t="s">
         <v>19</v>
@@ -3291,7 +3170,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="E19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F19" t="s">
         <v>19</v>
@@ -3302,10 +3181,10 @@
     </row>
     <row r="20" spans="1:10">
       <c r="E20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G20" t="b">
         <v>0</v>
@@ -3313,7 +3192,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="E21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F21" t="s">
         <v>20</v>
@@ -3324,7 +3203,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="E22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F22" t="s">
         <v>20</v>
@@ -3335,7 +3214,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="E23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F23" t="s">
         <v>20</v>
@@ -3346,7 +3225,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="E24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F24" t="s">
         <v>20</v>
@@ -3357,7 +3236,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="E25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F25" t="s">
         <v>19</v>
@@ -3368,7 +3247,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="E26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F26" t="s">
         <v>19</v>
@@ -3379,7 +3258,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="E27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F27" t="s">
         <v>20</v>
@@ -3402,13 +3281,13 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B29" t="s">
         <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D29" t="s">
         <v>14</v>
@@ -3419,7 +3298,7 @@
         <v>15</v>
       </c>
       <c r="E30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F30" t="s">
         <v>17</v>
@@ -3430,10 +3309,10 @@
     </row>
     <row r="31" spans="1:10">
       <c r="E31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G31" t="b">
         <v>0</v>
@@ -3441,7 +3320,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="E32" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F32" t="s">
         <v>20</v>
@@ -3452,7 +3331,7 @@
     </row>
     <row r="33" spans="5:7">
       <c r="E33" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F33" t="s">
         <v>20</v>
@@ -3463,7 +3342,7 @@
     </row>
     <row r="34" spans="5:7">
       <c r="E34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F34" t="s">
         <v>20</v>
@@ -3474,7 +3353,7 @@
     </row>
     <row r="35" spans="5:7">
       <c r="E35" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F35" t="s">
         <v>20</v>
@@ -3485,10 +3364,10 @@
     </row>
     <row r="36" spans="5:7">
       <c r="E36" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G36" t="b">
         <v>0</v>
@@ -3496,7 +3375,7 @@
     </row>
     <row r="37" spans="5:7">
       <c r="E37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F37" t="s">
         <v>19</v>
@@ -3507,7 +3386,7 @@
     </row>
     <row r="38" spans="5:7">
       <c r="E38" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F38" t="s">
         <v>19</v>
@@ -3518,10 +3397,10 @@
     </row>
     <row r="39" spans="5:7">
       <c r="E39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G39" t="b">
         <v>0</v>
@@ -3529,7 +3408,7 @@
     </row>
     <row r="40" spans="5:7">
       <c r="E40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F40" t="s">
         <v>20</v>
@@ -3540,7 +3419,7 @@
     </row>
     <row r="41" spans="5:7">
       <c r="E41" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F41" t="s">
         <v>20</v>
@@ -3551,7 +3430,7 @@
     </row>
     <row r="42" spans="5:7">
       <c r="E42" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F42" t="s">
         <v>20</v>
@@ -3562,10 +3441,10 @@
     </row>
     <row r="43" spans="5:7">
       <c r="E43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G43" t="b">
         <v>0</v>
@@ -3573,7 +3452,7 @@
     </row>
     <row r="44" spans="5:7">
       <c r="E44" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F44" t="s">
         <v>20</v>
@@ -3584,7 +3463,7 @@
     </row>
     <row r="45" spans="5:7">
       <c r="E45" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F45" t="s">
         <v>20</v>
@@ -3595,7 +3474,7 @@
     </row>
     <row r="46" spans="5:7">
       <c r="E46" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F46" t="s">
         <v>20</v>
@@ -3606,10 +3485,10 @@
     </row>
     <row r="47" spans="5:7">
       <c r="E47" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G47" t="b">
         <v>0</v>
@@ -3617,7 +3496,7 @@
     </row>
     <row r="48" spans="5:7">
       <c r="E48" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F48" t="s">
         <v>20</v>
@@ -3628,7 +3507,7 @@
     </row>
     <row r="49" spans="1:10">
       <c r="E49" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F49" t="s">
         <v>19</v>
@@ -3639,7 +3518,7 @@
     </row>
     <row r="50" spans="1:10">
       <c r="E50" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F50" t="s">
         <v>19</v>
@@ -3650,10 +3529,10 @@
     </row>
     <row r="51" spans="1:10">
       <c r="E51" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F51" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G51" t="b">
         <v>0</v>
@@ -3661,7 +3540,7 @@
     </row>
     <row r="52" spans="1:10">
       <c r="E52" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F52" t="s">
         <v>20</v>
@@ -3672,7 +3551,7 @@
     </row>
     <row r="53" spans="1:10">
       <c r="E53" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F53" t="s">
         <v>20</v>
@@ -3683,7 +3562,7 @@
     </row>
     <row r="54" spans="1:10">
       <c r="E54" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F54" t="s">
         <v>20</v>
@@ -3694,7 +3573,7 @@
     </row>
     <row r="55" spans="1:10">
       <c r="E55" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F55" t="s">
         <v>20</v>
@@ -3705,7 +3584,7 @@
     </row>
     <row r="56" spans="1:10">
       <c r="E56" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F56" t="s">
         <v>19</v>
@@ -3716,7 +3595,7 @@
     </row>
     <row r="57" spans="1:10">
       <c r="E57" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F57" t="s">
         <v>19</v>
@@ -3727,7 +3606,7 @@
     </row>
     <row r="58" spans="1:10">
       <c r="E58" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F58" t="s">
         <v>20</v>
@@ -3750,19 +3629,19 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B60" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C60" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D60" t="s">
         <v>14</v>
       </c>
       <c r="E60" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F60" t="s">
         <v>20</v>
@@ -3776,7 +3655,7 @@
         <v>15</v>
       </c>
       <c r="E61" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F61" t="s">
         <v>11</v>
@@ -3787,7 +3666,7 @@
     </row>
     <row r="62" spans="1:10">
       <c r="E62" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F62" t="s">
         <v>20</v>
@@ -3810,19 +3689,19 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B64" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C64" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D64" t="s">
         <v>14</v>
       </c>
       <c r="E64" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F64" t="s">
         <v>20</v>
@@ -3836,7 +3715,7 @@
         <v>15</v>
       </c>
       <c r="E65" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F65" t="s">
         <v>11</v>
@@ -3847,7 +3726,7 @@
     </row>
     <row r="66" spans="1:10">
       <c r="E66" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F66" t="s">
         <v>20</v>
@@ -3870,19 +3749,19 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B68" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C68" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D68" t="s">
         <v>14</v>
       </c>
       <c r="E68" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F68" t="s">
         <v>20</v>
@@ -3896,7 +3775,7 @@
         <v>15</v>
       </c>
       <c r="E69" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F69" t="s">
         <v>11</v>
@@ -3907,7 +3786,7 @@
     </row>
     <row r="70" spans="1:10">
       <c r="E70" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F70" t="s">
         <v>20</v>
@@ -3930,22 +3809,22 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B72" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C72" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D72" t="s">
         <v>14</v>
       </c>
       <c r="E72" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F72" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G72" t="b">
         <v>0</v>
@@ -3953,7 +3832,7 @@
     </row>
     <row r="73" spans="1:10">
       <c r="E73" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F73" t="s">
         <v>11</v>
@@ -3964,7 +3843,7 @@
     </row>
     <row r="74" spans="1:10">
       <c r="E74" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F74" t="s">
         <v>20</v>
@@ -3978,7 +3857,7 @@
         <v>15</v>
       </c>
       <c r="E75" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F75" t="s">
         <v>11</v>
@@ -3989,7 +3868,7 @@
     </row>
     <row r="76" spans="1:10">
       <c r="E76" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F76" t="s">
         <v>20</v>
@@ -4072,18 +3951,18 @@
         <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16" thickTop="1">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -4094,10 +3973,10 @@
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -4105,7 +3984,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="E4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
@@ -4116,7 +3995,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="E5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
@@ -4127,7 +4006,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="E6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
@@ -4138,7 +4017,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="E7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
@@ -4149,7 +4028,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="E8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
@@ -4160,7 +4039,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="E9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
@@ -4171,7 +4050,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="E10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
@@ -4182,7 +4061,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="E11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
@@ -4193,7 +4072,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="E12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
@@ -4204,7 +4083,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="E13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F13" t="s">
         <v>19</v>
@@ -4227,22 +4106,22 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
@@ -4250,7 +4129,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="E16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F16" t="s">
         <v>20</v>
@@ -4261,7 +4140,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="E17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F17" t="s">
         <v>20</v>
@@ -4272,7 +4151,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="E18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F18" t="s">
         <v>20</v>
@@ -4283,7 +4162,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="E19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F19" t="s">
         <v>20</v>
@@ -4294,7 +4173,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="E20" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F20" t="s">
         <v>20</v>
@@ -4305,7 +4184,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="E21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F21" t="s">
         <v>20</v>
@@ -4316,7 +4195,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="E22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F22" t="s">
         <v>20</v>
@@ -4327,7 +4206,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="E23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F23" t="s">
         <v>11</v>
@@ -4341,7 +4220,7 @@
         <v>15</v>
       </c>
       <c r="E24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F24" t="s">
         <v>11</v>
@@ -4352,7 +4231,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="E25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F25" t="s">
         <v>20</v>
@@ -4435,24 +4314,24 @@
         <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16" thickTop="1">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
@@ -4461,12 +4340,12 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="E3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -4477,7 +4356,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="E4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
@@ -4491,7 +4370,7 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -4502,7 +4381,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="E6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
@@ -4525,19 +4404,19 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
@@ -4548,7 +4427,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="E9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
@@ -4562,7 +4441,7 @@
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
@@ -4573,7 +4452,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="E11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
@@ -4596,13 +4475,13 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
@@ -4613,7 +4492,7 @@
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
         <v>11</v>
@@ -4624,7 +4503,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="E15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F15" t="s">
         <v>20</v>

</xml_diff>